<commit_message>
modified some code and scripts to add timestamps to maybe predict sr inflation
</commit_message>
<xml_diff>
--- a/TemplateTEC.xlsx
+++ b/TemplateTEC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9157321629fa917b/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\TECSRCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{77548EA3-CF12-4BFA-9A37-ED477BC45E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5BFFD9A-58CA-416A-957C-7E9F188944BF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A1D283-33F7-4D20-8BB2-689920429E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="6165" windowWidth="21600" windowHeight="11835" xr2:uid="{A460A165-F1AC-4A7F-8AFC-879A40BD8521}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A460A165-F1AC-4A7F-8AFC-879A40BD8521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>DPM</t>
   </si>
@@ -46,18 +46,27 @@
   <si>
     <t>SR</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4C4F69"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,13 +89,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -100,9 +116,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98FEE7D3-BCCF-44C3-9246-BC308682456A}" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{98FEE7D3-BCCF-44C3-9246-BC308682456A}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98FEE7D3-BCCF-44C3-9246-BC308682456A}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{98FEE7D3-BCCF-44C3-9246-BC308682456A}"/>
+  <tableColumns count="4">
+    <tableColumn id="4" xr3:uid="{D44701EE-5D4C-48CA-A896-4BF840BF80D0}" name="Date" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{6FFB1CDF-3EC8-458A-AEE6-0AFA0BA6BE3E}" name="DPM"/>
     <tableColumn id="2" xr3:uid="{786A08F1-6E93-41CB-8061-7979DC0398DE}" name="APM"/>
     <tableColumn id="3" xr3:uid="{0E9B8670-2CC3-40E9-B311-1C1F2E98C790}" name="SR"/>
@@ -428,23 +445,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA39E322-02C2-42DF-8E57-004E37E452DC}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>